<commit_message>
fix tests; rename MetaKey, MetaValue -> Attribute, Value
</commit_message>
<xml_diff>
--- a/test/resources/AutoCalc_Soccer_EventLog_FOR_REPLACE.xlsx
+++ b/test/resources/AutoCalc_Soccer_EventLog_FOR_REPLACE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="0" windowWidth="18120" windowHeight="14160" activeTab="1"/>
+    <workbookView xWindow="105" yWindow="0" windowWidth="18120" windowHeight="13890"/>
   </bookViews>
   <sheets>
     <sheet name="EventType" sheetId="4" r:id="rId1"/>
@@ -261,12 +261,6 @@
     <t>EventType</t>
   </si>
   <si>
-    <t>MetaKey</t>
-  </si>
-  <si>
-    <t>MetaValue</t>
-  </si>
-  <si>
     <t>Red Card</t>
   </si>
   <si>
@@ -364,6 +358,12 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -1041,7 +1041,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1051,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,16 +1066,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>69</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>71</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1173,7 +1173,7 @@
         <v>67</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1254,7 +1254,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D14" s="37" t="s">
         <v>68</v>
@@ -1262,7 +1262,7 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C15" s="40" t="s">
         <v>66</v>
@@ -1273,7 +1273,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C16" s="40" t="s">
         <v>66</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" s="40" t="s">
         <v>67</v>
@@ -1295,7 +1295,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>67</v>
@@ -1306,7 +1306,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C19" s="40" t="s">
         <v>67</v>
@@ -1317,7 +1317,7 @@
     </row>
     <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C20" s="41" t="s">
         <v>67</v>
@@ -1532,7 +1532,7 @@
         <v>67</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1540,10 +1540,10 @@
         <v>57</v>
       </c>
       <c r="C40" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1551,10 +1551,10 @@
         <v>57</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1562,10 +1562,10 @@
         <v>58</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1576,10 +1576,10 @@
         <v>58</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1590,10 +1590,10 @@
         <v>59</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1604,10 +1604,10 @@
         <v>59</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1618,10 +1618,10 @@
         <v>60</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1629,87 +1629,87 @@
         <v>60</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" s="38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C52" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C53" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" s="38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C54" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1717,13 +1717,13 @@
         <v>1</v>
       </c>
       <c r="B55" s="38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C55" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1742,7 +1742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17:G17"/>
     </sheetView>
   </sheetViews>
@@ -1775,10 +1775,10 @@
         <v>65</v>
       </c>
       <c r="F1" s="40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G1" s="39" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H1" s="34"/>
       <c r="I1" s="2"/>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -1820,7 +1820,7 @@
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H3" s="34"/>
       <c r="I3" s="2"/>
@@ -1835,10 +1835,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -1852,7 +1852,7 @@
         <v>57</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
@@ -1962,7 +1962,7 @@
         <v>57</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -1976,7 +1976,7 @@
         <v>58</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2095,10 +2095,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H18" s="34"/>
       <c r="I18" s="2"/>
@@ -2109,10 +2109,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -2123,14 +2123,14 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
       <c r="F20" s="25"/>
       <c r="G20" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="2"/>
@@ -2730,10 +2730,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2752,7 +2752,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="2">
         <f>COUNTIFS(EventLog!A:A,"Goal")</f>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B8" s="2">
         <f>COUNTIFS(EventLog!A:A,"YellowCard")</f>
@@ -2802,7 +2802,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B9" s="2">
         <f>COUNTIFS(EventLog!A:A,"Corner")</f>
@@ -2819,7 +2819,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11" s="2">
         <f>COUNTIFS(EventLog!A:A,"Goal",EventLog!B:B,"Team1", EventLog!C:C,"Half1")</f>
@@ -2830,7 +2830,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B12" s="2">
         <f>COUNTIFS(EventLog!A:A,"Goal",EventLog!B:B,"Team2", EventLog!C:C,"Half1")</f>
@@ -2847,7 +2847,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B14" s="2">
         <f>COUNTIFS(EventLog!A:A,"Goal",EventLog!B:B,"Team1", EventLog!C:C,"Half2")</f>
@@ -2858,7 +2858,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B15" s="2">
         <f>COUNTIFS(EventLog!A:A,"Goal",EventLog!B:B,"Team2", EventLog!C:C,"Half2")</f>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B17" s="2">
         <f>COUNTIFS(EventLog!A:A,"Goal",G:G, "&lt;&gt;")</f>
@@ -2892,7 +2892,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B19" s="2">
         <f>COUNTIFS(EventLog!A:A,"Goal",H:H, "Head")</f>
@@ -2909,7 +2909,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B21" s="2" t="b">
         <f>IF(COUNTIFS(EventLog!A:A,"Goal",EventLog!C:C,"Half1",B:B,"&gt;0",B:B,"&lt;15"), TRUE,FALSE)</f>
@@ -2920,7 +2920,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22" s="2" t="b">
         <f>IF(COUNTIFS(EventLog!A:A,"Goal",EventLog!C:C,"Half1",B:B,"&gt;15",B:B,"&lt;30"), TRUE,FALSE)</f>
@@ -2937,7 +2937,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B24" s="2" t="b">
         <f>COUNTIFS(EventLog!A:A,"Match",EventLog!G:G,"stop")&gt;0</f>
@@ -2948,7 +2948,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B25" s="2" t="b">
         <f>COUNTIFS(EventLog!A:A,"Half1",EventLog!G:G,"stop")&gt;0</f>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B27" s="2" t="e">
         <f>0&lt;INDEX(EventLog!#REF!,MATCH("Goal",EventLog!A:A,0))&lt;15</f>
@@ -2976,7 +2976,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B28" s="2" t="e">
         <f>AND(15&lt;INDEX(EventLog!#REF!,MATCH("Goal",EventLog!A:A,0)),30&gt;INDEX(EventLog!#REF!,MATCH("Goal",EventLog!A:A,0)))</f>
@@ -2993,7 +2993,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B30" s="2" t="str">
         <f t="array" ref="B30">INDEX(EventLog!B:B,SMALL(IF(EventLog!A:A="Goal",ROW(EventLog!A:A),""),2))</f>
@@ -3004,7 +3004,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B31" s="2" t="e">
         <f t="array" ref="B31">INDEX(EventLog!#REF!,SMALL(IF(EventLog!A:A="Goal",ROW(EventLog!A:A),""),3))</f>

</xml_diff>